<commit_message>
docs: add detailed error management
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111OLOMEDIAXXX/Olomedia/oloHealth/V.3.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111OLOMEDIAXXX/Olomedia/oloHealth/V.3.0.0/report-checklist.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="452">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -519,7 +519,7 @@
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">Verifica dei log ed eventuale reinvio</t>
+    <t xml:space="preserve">In caso di JWT errato il processo applicativo prosegue ed il documento viene firmato. Il documento sarà inserito in coda e tenterà un nuovo tentativo di validazione. Viene messo a disposizione una reportistica sulla verifica dei documenti che hanno avuto errori di validazione da parte del gateway per poterli individuare.</t>
   </si>
   <si>
     <t xml:space="preserve">KO</t>
@@ -587,7 +587,7 @@
 Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nella colonna "J" nominata come "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t xml:space="preserve">Richiesta annullata: Timeout dell’operazione</t>
+    <t xml:space="preserve">In caso di timeout il processo applicativo prosegue ed il documento viene firmato. Il documento sarà inserito in coda e tenterà un nuovo tentativo di validazione. Viene messo a disposizione una reportistica sulla verifica dei documenti che hanno avuto errori di validazione da parte del gateway per poterli individuare.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_RSA_TIMEOUT</t>
@@ -613,6 +613,12 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.4.81bd8aa200f40537a18b16f0328146fc5c2f0515dfa45e84e4d58ee230e7aba8.eea0faf3b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
+    <t xml:space="preserve">Verificare dati errati o mancanti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il processo di firma viene interrotto mostrando all'utente un messaggio d'errore relativo al campo indicato, invintando l'operatore alla selezione di un valore possibile tra quelli presenti nell'elenco. Solo al termine del corretto inserimento dei dati relativi al messaggio d'errore il documento viene inviato al FSE per la validazione.</t>
+  </si>
+  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT6_KO</t>
   </si>
   <si>
@@ -911,6 +917,12 @@
   </si>
   <si>
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.4.4003cd725a780165cde9dbd9892ea3f5411c3b23e99e33e6fc9c81fec848158c.e27e338e40^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si e’ verificato un errore imprevisto. Riprovare piu tardi o contattare il supporto tecnico.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'errore viene segnalato all'utente che viene invitato a riprovare o a contattare l'help desk. Il servizio di manutenzione software risolve gli errori giornalmente. Dopo la risoluzione, il medico riprende il processo documentale e invia il documento per la validazione. Se possibile, gli operatori correggono l'errore e ri-validano il documento. Altrimenti, il processo clinico continua e il documento viene rivalidato successivamente. Se il gateway non è disponibile, il documento viene memorizzato e inviato in seguito.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_VPS_CT12_KO</t>
@@ -1680,7 +1692,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1772,6 +1784,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1892,7 +1910,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2010,6 +2028,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2155,11 +2177,11 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="9:9 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.89"/>
@@ -3229,11 +3251,11 @@
   </sheetPr>
   <dimension ref="A1:B998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="9:9 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.11"/>
@@ -4336,15 +4358,15 @@
   </sheetPr>
   <dimension ref="A1:T704"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B9" activeCellId="0" sqref="9:9"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.09"/>
@@ -4945,7 +4967,7 @@
       <c r="O18" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P18" s="27" t="s">
+      <c r="P18" s="16" t="s">
         <v>100</v>
       </c>
       <c r="Q18" s="27" t="s">
@@ -4992,7 +5014,7 @@
       <c r="O19" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P19" s="27" t="s">
+      <c r="P19" s="16" t="s">
         <v>100</v>
       </c>
       <c r="Q19" s="27" t="s">
@@ -5039,7 +5061,7 @@
       <c r="O20" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P20" s="27" t="s">
+      <c r="P20" s="16" t="s">
         <v>100</v>
       </c>
       <c r="Q20" s="27" t="s">
@@ -5086,7 +5108,7 @@
       <c r="O21" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P21" s="27" t="s">
+      <c r="P21" s="16" t="s">
         <v>100</v>
       </c>
       <c r="Q21" s="27" t="s">
@@ -5133,7 +5155,7 @@
       <c r="O22" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P22" s="27" t="s">
+      <c r="P22" s="16" t="s">
         <v>100</v>
       </c>
       <c r="Q22" s="27" t="s">
@@ -5180,7 +5202,7 @@
       <c r="O23" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P23" s="27" t="s">
+      <c r="P23" s="16" t="s">
         <v>100</v>
       </c>
       <c r="Q23" s="27" t="s">
@@ -5190,7 +5212,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" s="27" customFormat="true" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="27" customFormat="true" ht="120.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="n">
         <v>45</v>
       </c>
@@ -5212,7 +5234,16 @@
       <c r="J24" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P24" s="27" t="s">
+      <c r="L24" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M24" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="O24" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="P24" s="16" t="s">
         <v>121</v>
       </c>
       <c r="Q24" s="27" t="s">
@@ -5225,7 +5256,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" s="27" customFormat="true" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="27" customFormat="true" ht="120.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="n">
         <v>48</v>
       </c>
@@ -5247,7 +5278,16 @@
       <c r="J25" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P25" s="27" t="s">
+      <c r="L25" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M25" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="O25" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="P25" s="16" t="s">
         <v>121</v>
       </c>
       <c r="Q25" s="27" t="s">
@@ -5260,7 +5300,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" s="27" customFormat="true" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="27" customFormat="true" ht="120.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="27" t="n">
         <v>51</v>
       </c>
@@ -5282,7 +5322,16 @@
       <c r="J26" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P26" s="27" t="s">
+      <c r="L26" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="O26" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" s="16" t="s">
         <v>121</v>
       </c>
       <c r="Q26" s="27" t="s">
@@ -5295,7 +5344,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27" t="n">
         <v>63</v>
       </c>
@@ -5327,16 +5376,19 @@
         <v>56</v>
       </c>
       <c r="L27" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N27" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O27" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M27" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O27" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P27" s="27" t="s">
-        <v>100</v>
+      <c r="P27" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q27" s="27" t="s">
         <v>57</v>
@@ -5345,7 +5397,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="27" t="n">
         <v>64</v>
       </c>
@@ -5356,37 +5408,40 @@
         <v>49</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F28" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J28" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L28" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N28" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O28" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M28" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O28" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P28" s="27" t="s">
-        <v>100</v>
+      <c r="P28" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q28" s="27" t="s">
         <v>57</v>
@@ -5395,7 +5450,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="27" t="n">
         <v>65</v>
       </c>
@@ -5406,37 +5461,40 @@
         <v>49</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F29" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J29" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L29" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O29" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M29" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O29" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P29" s="27" t="s">
-        <v>100</v>
+      <c r="P29" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q29" s="27" t="s">
         <v>57</v>
@@ -5445,7 +5503,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="27" t="n">
         <v>66</v>
       </c>
@@ -5456,22 +5514,22 @@
         <v>49</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F30" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H30" s="27" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J30" s="27" t="s">
         <v>56</v>
@@ -5480,13 +5538,16 @@
         <v>56</v>
       </c>
       <c r="M30" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N30" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O30" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="O30" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P30" s="27" t="s">
-        <v>100</v>
+      <c r="P30" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q30" s="27" t="s">
         <v>57</v>
@@ -5495,7 +5556,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="27" t="n">
         <v>67</v>
       </c>
@@ -5506,22 +5567,22 @@
         <v>49</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F31" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H31" s="27" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J31" s="27" t="s">
         <v>56</v>
@@ -5530,13 +5591,16 @@
         <v>56</v>
       </c>
       <c r="M31" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N31" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O31" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="O31" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P31" s="27" t="s">
-        <v>100</v>
+      <c r="P31" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q31" s="27" t="s">
         <v>57</v>
@@ -5545,7 +5609,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="27" t="n">
         <v>68</v>
       </c>
@@ -5556,22 +5620,22 @@
         <v>49</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F32" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H32" s="27" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J32" s="27" t="s">
         <v>56</v>
@@ -5580,13 +5644,16 @@
         <v>56</v>
       </c>
       <c r="M32" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N32" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O32" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="O32" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P32" s="27" t="s">
-        <v>100</v>
+      <c r="P32" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q32" s="27" t="s">
         <v>57</v>
@@ -5595,7 +5662,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="27" t="n">
         <v>69</v>
       </c>
@@ -5606,22 +5673,22 @@
         <v>49</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F33" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H33" s="27" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I33" s="27" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J33" s="27" t="s">
         <v>56</v>
@@ -5630,13 +5697,16 @@
         <v>56</v>
       </c>
       <c r="M33" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N33" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O33" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="O33" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P33" s="27" t="s">
-        <v>100</v>
+      <c r="P33" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q33" s="27" t="s">
         <v>57</v>
@@ -5645,7 +5715,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="27" t="n">
         <v>70</v>
       </c>
@@ -5656,22 +5726,22 @@
         <v>49</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F34" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H34" s="27" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I34" s="27" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J34" s="27" t="s">
         <v>56</v>
@@ -5680,13 +5750,16 @@
         <v>56</v>
       </c>
       <c r="M34" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N34" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O34" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="O34" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P34" s="27" t="s">
-        <v>100</v>
+      <c r="P34" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q34" s="27" t="s">
         <v>57</v>
@@ -5695,7 +5768,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="27" t="n">
         <v>71</v>
       </c>
@@ -5706,22 +5779,22 @@
         <v>49</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F35" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H35" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I35" s="27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="J35" s="27" t="s">
         <v>56</v>
@@ -5730,13 +5803,16 @@
         <v>56</v>
       </c>
       <c r="M35" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N35" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O35" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="O35" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P35" s="27" t="s">
-        <v>100</v>
+      <c r="P35" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q35" s="27" t="s">
         <v>57</v>
@@ -5745,7 +5821,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="27" t="n">
         <v>72</v>
       </c>
@@ -5756,22 +5832,22 @@
         <v>49</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F36" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H36" s="27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I36" s="27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J36" s="27" t="s">
         <v>56</v>
@@ -5780,13 +5856,16 @@
         <v>56</v>
       </c>
       <c r="M36" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N36" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O36" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="O36" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P36" s="27" t="s">
-        <v>100</v>
+      <c r="P36" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q36" s="27" t="s">
         <v>57</v>
@@ -5795,7 +5874,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="27" t="n">
         <v>73</v>
       </c>
@@ -5806,37 +5885,40 @@
         <v>49</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F37" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H37" s="27" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J37" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L37" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M37" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N37" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O37" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M37" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O37" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P37" s="27" t="s">
-        <v>100</v>
+      <c r="P37" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q37" s="27" t="s">
         <v>57</v>
@@ -5845,7 +5927,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="27" t="n">
         <v>74</v>
       </c>
@@ -5856,37 +5938,40 @@
         <v>49</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F38" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H38" s="27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="I38" s="27" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="J38" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L38" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M38" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N38" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O38" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M38" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O38" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P38" s="27" t="s">
-        <v>100</v>
+      <c r="P38" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q38" s="27" t="s">
         <v>57</v>
@@ -5895,7 +5980,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="27" t="n">
         <v>122</v>
       </c>
@@ -5906,37 +5991,40 @@
         <v>74</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F39" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H39" s="27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I39" s="27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="J39" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L39" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N39" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O39" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M39" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O39" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P39" s="27" t="s">
-        <v>100</v>
+      <c r="P39" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q39" s="27" t="s">
         <v>57</v>
@@ -5945,7 +6033,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="27" t="n">
         <v>123</v>
       </c>
@@ -5956,37 +6044,40 @@
         <v>74</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F40" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H40" s="27" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J40" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L40" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M40" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N40" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O40" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M40" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O40" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P40" s="27" t="s">
-        <v>100</v>
+      <c r="P40" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q40" s="27" t="s">
         <v>57</v>
@@ -5995,7 +6086,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="27" t="n">
         <v>124</v>
       </c>
@@ -6006,37 +6097,40 @@
         <v>74</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F41" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H41" s="27" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I41" s="27" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J41" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L41" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M41" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N41" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O41" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M41" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O41" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P41" s="27" t="s">
-        <v>100</v>
+      <c r="P41" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q41" s="27" t="s">
         <v>57</v>
@@ -6045,7 +6139,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="27" t="n">
         <v>125</v>
       </c>
@@ -6056,37 +6150,40 @@
         <v>74</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F42" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H42" s="27" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I42" s="27" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J42" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L42" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M42" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N42" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O42" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M42" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O42" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P42" s="27" t="s">
-        <v>100</v>
+      <c r="P42" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q42" s="27" t="s">
         <v>57</v>
@@ -6095,7 +6192,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="27" t="n">
         <v>126</v>
       </c>
@@ -6106,37 +6203,40 @@
         <v>74</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H43" s="27" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I43" s="27" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="J43" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L43" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M43" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N43" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O43" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M43" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O43" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P43" s="27" t="s">
-        <v>100</v>
+      <c r="P43" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q43" s="27" t="s">
         <v>57</v>
@@ -6145,7 +6245,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="27" t="n">
         <v>127</v>
       </c>
@@ -6156,37 +6256,40 @@
         <v>74</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F44" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H44" s="27" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J44" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L44" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M44" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N44" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O44" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M44" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O44" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P44" s="27" t="s">
-        <v>100</v>
+      <c r="P44" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q44" s="27" t="s">
         <v>57</v>
@@ -6195,7 +6298,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="27" t="n">
         <v>128</v>
       </c>
@@ -6206,37 +6309,40 @@
         <v>74</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F45" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H45" s="27" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I45" s="27" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J45" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L45" s="27" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="M45" s="27" t="s">
-        <v>99</v>
+        <v>56</v>
+      </c>
+      <c r="N45" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="O45" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P45" s="27" t="s">
-        <v>100</v>
+      <c r="P45" s="16" t="s">
+        <v>222</v>
       </c>
       <c r="Q45" s="27" t="s">
         <v>57</v>
@@ -6245,7 +6351,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="27" t="n">
         <v>129</v>
       </c>
@@ -6256,37 +6362,40 @@
         <v>74</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F46" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G46" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="H46" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="I46" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="J46" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="L46" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M46" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N46" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="H46" s="27" t="s">
+      <c r="O46" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="P46" s="16" t="s">
         <v>222</v>
-      </c>
-      <c r="I46" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="J46" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="L46" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="M46" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O46" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P46" s="27" t="s">
-        <v>100</v>
       </c>
       <c r="Q46" s="27" t="s">
         <v>57</v>
@@ -6295,7 +6404,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="27" t="n">
         <v>130</v>
       </c>
@@ -6306,37 +6415,40 @@
         <v>74</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F47" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="H47" s="27" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="I47" s="27" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="J47" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L47" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M47" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N47" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O47" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M47" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O47" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P47" s="27" t="s">
-        <v>100</v>
+      <c r="P47" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q47" s="27" t="s">
         <v>57</v>
@@ -6345,7 +6457,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="27" t="n">
         <v>131</v>
       </c>
@@ -6356,37 +6468,40 @@
         <v>74</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="F48" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="H48" s="27" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="I48" s="27" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="J48" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L48" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M48" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N48" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O48" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M48" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O48" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P48" s="27" t="s">
-        <v>100</v>
+      <c r="P48" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q48" s="27" t="s">
         <v>57</v>
@@ -6395,7 +6510,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="27" t="n">
         <v>132</v>
       </c>
@@ -6406,37 +6521,40 @@
         <v>74</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="F49" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I49" s="27" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="J49" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L49" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M49" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N49" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O49" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M49" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O49" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P49" s="27" t="s">
-        <v>100</v>
+      <c r="P49" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q49" s="27" t="s">
         <v>57</v>
@@ -6445,7 +6563,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="27" t="n">
         <v>133</v>
       </c>
@@ -6456,37 +6574,40 @@
         <v>74</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="F50" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="J50" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L50" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M50" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N50" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O50" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M50" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O50" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P50" s="27" t="s">
-        <v>100</v>
+      <c r="P50" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q50" s="27" t="s">
         <v>57</v>
@@ -6495,7 +6616,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="27" t="n">
         <v>134</v>
       </c>
@@ -6506,37 +6627,40 @@
         <v>74</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F51" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="I51" s="27" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="J51" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L51" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M51" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N51" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O51" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M51" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O51" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P51" s="27" t="s">
-        <v>100</v>
+      <c r="P51" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q51" s="27" t="s">
         <v>57</v>
@@ -6545,7 +6669,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="27" t="n">
         <v>135</v>
       </c>
@@ -6556,37 +6680,40 @@
         <v>74</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F52" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I52" s="27" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="J52" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L52" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M52" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N52" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O52" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M52" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O52" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P52" s="27" t="s">
-        <v>100</v>
+      <c r="P52" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q52" s="27" t="s">
         <v>57</v>
@@ -6595,7 +6722,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="27" t="n">
         <v>136</v>
       </c>
@@ -6606,37 +6733,40 @@
         <v>74</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F53" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="I53" s="27" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="J53" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L53" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M53" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N53" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O53" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M53" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O53" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P53" s="27" t="s">
-        <v>100</v>
+      <c r="P53" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q53" s="27" t="s">
         <v>57</v>
@@ -6645,7 +6775,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="27" t="n">
         <v>137</v>
       </c>
@@ -6656,37 +6786,40 @@
         <v>74</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="F54" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="H54" s="27" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I54" s="27" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="J54" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L54" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M54" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N54" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O54" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M54" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O54" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P54" s="27" t="s">
-        <v>100</v>
+      <c r="P54" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q54" s="27" t="s">
         <v>57</v>
@@ -6695,7 +6828,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="55" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="27" t="n">
         <v>138</v>
       </c>
@@ -6706,37 +6839,40 @@
         <v>74</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="F55" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H55" s="27" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="J55" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L55" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M55" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N55" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O55" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M55" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O55" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P55" s="27" t="s">
-        <v>100</v>
+      <c r="P55" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q55" s="27" t="s">
         <v>57</v>
@@ -6745,7 +6881,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="27" t="n">
         <v>139</v>
       </c>
@@ -6756,37 +6892,40 @@
         <v>74</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="F56" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G56" s="27" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="H56" s="27" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="I56" s="27" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="J56" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L56" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M56" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N56" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O56" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M56" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O56" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P56" s="27" t="s">
-        <v>100</v>
+      <c r="P56" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q56" s="27" t="s">
         <v>57</v>
@@ -6795,7 +6934,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="27" t="n">
         <v>140</v>
       </c>
@@ -6806,37 +6945,40 @@
         <v>74</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F57" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G57" s="27" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="H57" s="27" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I57" s="27" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="J57" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L57" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M57" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N57" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O57" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M57" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O57" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P57" s="27" t="s">
-        <v>100</v>
+      <c r="P57" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q57" s="27" t="s">
         <v>57</v>
@@ -6845,7 +6987,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="27" t="n">
         <v>141</v>
       </c>
@@ -6856,37 +6998,40 @@
         <v>74</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="F58" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G58" s="27" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="H58" s="27" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="I58" s="27" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="J58" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L58" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M58" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N58" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O58" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M58" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O58" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P58" s="27" t="s">
-        <v>100</v>
+      <c r="P58" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q58" s="27" t="s">
         <v>57</v>
@@ -6895,7 +7040,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="27" t="n">
         <v>142</v>
       </c>
@@ -6906,37 +7051,40 @@
         <v>74</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F59" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G59" s="27" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="H59" s="27" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="I59" s="27" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="J59" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L59" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M59" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N59" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O59" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M59" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O59" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P59" s="27" t="s">
-        <v>100</v>
+      <c r="P59" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q59" s="27" t="s">
         <v>57</v>
@@ -6945,7 +7093,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="27" t="n">
         <v>143</v>
       </c>
@@ -6956,37 +7104,40 @@
         <v>74</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F60" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G60" s="27" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="H60" s="27" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="I60" s="27" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="J60" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L60" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M60" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N60" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O60" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M60" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O60" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P60" s="27" t="s">
-        <v>100</v>
+      <c r="P60" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q60" s="27" t="s">
         <v>57</v>
@@ -6995,7 +7146,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="27" t="n">
         <v>144</v>
       </c>
@@ -7006,37 +7157,40 @@
         <v>74</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E61" s="28" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="F61" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G61" s="27" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="H61" s="27" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="I61" s="27" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="J61" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L61" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M61" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N61" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O61" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M61" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O61" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P61" s="27" t="s">
-        <v>100</v>
+      <c r="P61" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q61" s="27" t="s">
         <v>57</v>
@@ -7045,7 +7199,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="27" t="n">
         <v>145</v>
       </c>
@@ -7056,37 +7210,40 @@
         <v>74</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="E62" s="28" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="F62" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G62" s="27" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H62" s="27" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="J62" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L62" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M62" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N62" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O62" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M62" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O62" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P62" s="27" t="s">
-        <v>100</v>
+      <c r="P62" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q62" s="27" t="s">
         <v>57</v>
@@ -7095,7 +7252,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="27" t="n">
         <v>146</v>
       </c>
@@ -7106,37 +7263,40 @@
         <v>74</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="F63" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G63" s="27" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="H63" s="27" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="I63" s="27" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="J63" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L63" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M63" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N63" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O63" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M63" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O63" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P63" s="27" t="s">
-        <v>100</v>
+      <c r="P63" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q63" s="27" t="s">
         <v>57</v>
@@ -7145,7 +7305,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" s="27" customFormat="true" ht="199.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" s="27" customFormat="true" ht="187.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="27" t="n">
         <v>147</v>
       </c>
@@ -7156,22 +7316,22 @@
         <v>102</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="F64" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G64" s="27" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="H64" s="27" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="I64" s="27" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="J64" s="27" t="s">
         <v>56</v>
@@ -7183,7 +7343,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" s="27" customFormat="true" ht="199.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="27" customFormat="true" ht="187.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="27" t="n">
         <v>148</v>
       </c>
@@ -7194,22 +7354,22 @@
         <v>102</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="F65" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G65" s="27" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="H65" s="27" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="I65" s="27" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="J65" s="27" t="s">
         <v>56</v>
@@ -7221,7 +7381,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" s="27" customFormat="true" ht="199.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" s="27" customFormat="true" ht="187.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="27" t="n">
         <v>149</v>
       </c>
@@ -7232,22 +7392,22 @@
         <v>102</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="F66" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G66" s="27" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="H66" s="27" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="I66" s="27" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="J66" s="27" t="s">
         <v>56</v>
@@ -7259,7 +7419,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" s="27" customFormat="true" ht="199.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="27" customFormat="true" ht="187.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="27" t="n">
         <v>150</v>
       </c>
@@ -7270,22 +7430,22 @@
         <v>102</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F67" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G67" s="27" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="H67" s="27" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="I67" s="27" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="J67" s="27" t="s">
         <v>56</v>
@@ -7297,7 +7457,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="27" customFormat="true" ht="132.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="27" t="n">
         <v>151</v>
       </c>
@@ -7308,37 +7468,40 @@
         <v>102</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="F68" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G68" s="27" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="H68" s="27" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="I68" s="27" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="J68" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L68" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M68" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N68" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="O68" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M68" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O68" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P68" s="27" t="s">
-        <v>100</v>
+      <c r="P68" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q68" s="27" t="s">
         <v>57</v>
@@ -7347,7 +7510,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="27" t="n">
         <v>152</v>
       </c>
@@ -7358,37 +7521,40 @@
         <v>102</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="F69" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G69" s="27" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="H69" s="27" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="I69" s="27" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="J69" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L69" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M69" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N69" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O69" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M69" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O69" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P69" s="27" t="s">
-        <v>100</v>
+      <c r="P69" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q69" s="27" t="s">
         <v>57</v>
@@ -7397,7 +7563,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="27" t="n">
         <v>153</v>
       </c>
@@ -7408,37 +7574,40 @@
         <v>102</v>
       </c>
       <c r="D70" s="27" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="E70" s="28" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="F70" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G70" s="27" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="H70" s="27" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="I70" s="27" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="J70" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L70" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M70" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N70" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O70" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M70" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O70" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P70" s="27" t="s">
-        <v>100</v>
+      <c r="P70" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q70" s="27" t="s">
         <v>57</v>
@@ -7447,7 +7616,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="27" t="n">
         <v>154</v>
       </c>
@@ -7458,37 +7627,40 @@
         <v>102</v>
       </c>
       <c r="D71" s="27" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="F71" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G71" s="27" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="H71" s="27" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="J71" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L71" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M71" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N71" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O71" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M71" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O71" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P71" s="27" t="s">
-        <v>100</v>
+      <c r="P71" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q71" s="27" t="s">
         <v>57</v>
@@ -7497,7 +7669,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="27" t="n">
         <v>155</v>
       </c>
@@ -7508,37 +7680,40 @@
         <v>102</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F72" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G72" s="27" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="H72" s="27" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="I72" s="27" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="J72" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L72" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M72" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N72" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O72" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M72" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O72" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P72" s="27" t="s">
-        <v>100</v>
+      <c r="P72" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q72" s="27" t="s">
         <v>57</v>
@@ -7547,7 +7722,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="27" t="n">
         <v>156</v>
       </c>
@@ -7558,37 +7733,40 @@
         <v>102</v>
       </c>
       <c r="D73" s="27" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="F73" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G73" s="27" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="H73" s="27" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="I73" s="27" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="J73" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L73" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M73" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N73" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O73" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M73" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O73" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P73" s="27" t="s">
-        <v>100</v>
+      <c r="P73" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q73" s="27" t="s">
         <v>57</v>
@@ -7597,7 +7775,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="27" t="n">
         <v>157</v>
       </c>
@@ -7608,37 +7786,40 @@
         <v>102</v>
       </c>
       <c r="D74" s="27" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="F74" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G74" s="27" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="H74" s="27" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="I74" s="27" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="J74" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L74" s="27" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="M74" s="27" t="s">
-        <v>99</v>
+        <v>56</v>
+      </c>
+      <c r="N74" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="O74" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P74" s="27" t="s">
-        <v>100</v>
+      <c r="P74" s="16" t="s">
+        <v>222</v>
       </c>
       <c r="Q74" s="27" t="s">
         <v>57</v>
@@ -7647,7 +7828,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="75" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="27" t="n">
         <v>158</v>
       </c>
@@ -7658,37 +7839,40 @@
         <v>102</v>
       </c>
       <c r="D75" s="27" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="F75" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G75" s="27" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="H75" s="27" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="I75" s="27" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="J75" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L75" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M75" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N75" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O75" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M75" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O75" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P75" s="27" t="s">
-        <v>100</v>
+      <c r="P75" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q75" s="27" t="s">
         <v>57</v>
@@ -7697,7 +7881,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="76" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="27" t="n">
         <v>159</v>
       </c>
@@ -7708,37 +7892,40 @@
         <v>102</v>
       </c>
       <c r="D76" s="27" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="F76" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G76" s="27" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="H76" s="27" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="I76" s="27" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="J76" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L76" s="27" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="M76" s="27" t="s">
-        <v>99</v>
+        <v>56</v>
+      </c>
+      <c r="N76" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="O76" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P76" s="27" t="s">
-        <v>100</v>
+      <c r="P76" s="16" t="s">
+        <v>222</v>
       </c>
       <c r="Q76" s="27" t="s">
         <v>57</v>
@@ -7747,7 +7934,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="77" s="27" customFormat="true" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="27" t="n">
         <v>160</v>
       </c>
@@ -7758,37 +7945,40 @@
         <v>102</v>
       </c>
       <c r="D77" s="27" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F77" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G77" s="27" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="H77" s="27" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="I77" s="27" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="J77" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L77" s="27" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="M77" s="27" t="s">
-        <v>99</v>
+        <v>56</v>
+      </c>
+      <c r="N77" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="O77" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P77" s="27" t="s">
-        <v>100</v>
+      <c r="P77" s="16" t="s">
+        <v>222</v>
       </c>
       <c r="Q77" s="27" t="s">
         <v>57</v>
@@ -7797,7 +7987,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="27" t="n">
         <v>161</v>
       </c>
@@ -7808,37 +7998,40 @@
         <v>102</v>
       </c>
       <c r="D78" s="27" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="F78" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G78" s="27" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="H78" s="27" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="I78" s="27" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="J78" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L78" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M78" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N78" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O78" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M78" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O78" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P78" s="27" t="s">
-        <v>100</v>
+      <c r="P78" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q78" s="27" t="s">
         <v>57</v>
@@ -7847,7 +8040,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="79" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="27" t="n">
         <v>162</v>
       </c>
@@ -7858,37 +8051,40 @@
         <v>102</v>
       </c>
       <c r="D79" s="27" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="E79" s="28" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="F79" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G79" s="27" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="I79" s="27" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="J79" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L79" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M79" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N79" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O79" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M79" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O79" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P79" s="27" t="s">
-        <v>100</v>
+      <c r="P79" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q79" s="27" t="s">
         <v>57</v>
@@ -7897,7 +8093,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="27" t="n">
         <v>163</v>
       </c>
@@ -7908,37 +8104,40 @@
         <v>102</v>
       </c>
       <c r="D80" s="27" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="F80" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G80" s="27" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="H80" s="27" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="I80" s="27" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="J80" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L80" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M80" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N80" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O80" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M80" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O80" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P80" s="27" t="s">
-        <v>100</v>
+      <c r="P80" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q80" s="27" t="s">
         <v>57</v>
@@ -7947,7 +8146,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="27" t="n">
         <v>164</v>
       </c>
@@ -7958,37 +8157,40 @@
         <v>102</v>
       </c>
       <c r="D81" s="27" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="E81" s="28" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F81" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G81" s="27" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="H81" s="27" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="I81" s="27" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="J81" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L81" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M81" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N81" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O81" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M81" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O81" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P81" s="27" t="s">
-        <v>100</v>
+      <c r="P81" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q81" s="27" t="s">
         <v>57</v>
@@ -7997,7 +8199,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="82" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="27" t="n">
         <v>165</v>
       </c>
@@ -8008,37 +8210,40 @@
         <v>102</v>
       </c>
       <c r="D82" s="27" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="E82" s="28" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="F82" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G82" s="27" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="H82" s="27" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="I82" s="27" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="J82" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L82" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M82" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N82" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O82" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M82" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O82" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P82" s="27" t="s">
-        <v>100</v>
+      <c r="P82" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q82" s="27" t="s">
         <v>57</v>
@@ -8047,7 +8252,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="27" t="n">
         <v>166</v>
       </c>
@@ -8058,37 +8263,40 @@
         <v>102</v>
       </c>
       <c r="D83" s="27" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="E83" s="28" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="F83" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G83" s="27" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="H83" s="27" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="I83" s="27" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="J83" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L83" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M83" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N83" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O83" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M83" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O83" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P83" s="27" t="s">
-        <v>100</v>
+      <c r="P83" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q83" s="27" t="s">
         <v>57</v>
@@ -8097,7 +8305,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="84" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="27" t="n">
         <v>167</v>
       </c>
@@ -8108,37 +8316,40 @@
         <v>102</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="E84" s="28" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="F84" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G84" s="27" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="H84" s="27" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="I84" s="27" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="J84" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L84" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M84" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N84" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O84" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M84" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O84" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P84" s="27" t="s">
-        <v>100</v>
+      <c r="P84" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q84" s="27" t="s">
         <v>57</v>
@@ -8147,7 +8358,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="85" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="27" t="n">
         <v>168</v>
       </c>
@@ -8158,37 +8369,40 @@
         <v>102</v>
       </c>
       <c r="D85" s="27" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="E85" s="28" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="F85" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G85" s="27" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="H85" s="27" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="I85" s="27" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="J85" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L85" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M85" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N85" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O85" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M85" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O85" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P85" s="27" t="s">
-        <v>100</v>
+      <c r="P85" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q85" s="27" t="s">
         <v>57</v>
@@ -8197,7 +8411,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="86" s="27" customFormat="true" ht="153.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" s="27" customFormat="true" ht="147.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="27" t="n">
         <v>169</v>
       </c>
@@ -8208,37 +8422,40 @@
         <v>102</v>
       </c>
       <c r="D86" s="27" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="E86" s="28" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="F86" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G86" s="27" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="H86" s="27" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="I86" s="27" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="J86" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L86" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M86" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="N86" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O86" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="M86" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="O86" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P86" s="27" t="s">
-        <v>100</v>
+      <c r="P86" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="Q86" s="27" t="s">
         <v>57</v>
@@ -17873,13 +18090,13 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="9:9 A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.87"/>
@@ -17898,10 +18115,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17909,13 +18126,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>427</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>428</v>
+        <v>430</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>431</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17923,13 +18140,13 @@
         <v>49</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="C3" s="30" t="n">
+        <v>433</v>
+      </c>
+      <c r="C3" s="31" t="n">
         <v>208</v>
       </c>
-      <c r="D3" s="30" t="s">
-        <v>430</v>
+      <c r="D3" s="31" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17937,13 +18154,13 @@
         <v>49</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="C4" s="30" t="n">
+        <v>435</v>
+      </c>
+      <c r="C4" s="31" t="n">
         <v>209</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>432</v>
+      <c r="D4" s="31" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17951,13 +18168,13 @@
         <v>49</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="C5" s="30" t="n">
+        <v>437</v>
+      </c>
+      <c r="C5" s="31" t="n">
         <v>210</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>434</v>
+      <c r="D5" s="31" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17965,12 +18182,12 @@
         <v>49</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="C6" s="30" t="n">
+        <v>439</v>
+      </c>
+      <c r="C6" s="31" t="n">
         <v>211</v>
       </c>
-      <c r="D6" s="30" t="n">
+      <c r="D6" s="31" t="n">
         <v>220</v>
       </c>
     </row>
@@ -17979,12 +18196,12 @@
         <v>49</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="C7" s="30" t="n">
+        <v>440</v>
+      </c>
+      <c r="C7" s="31" t="n">
         <v>212</v>
       </c>
-      <c r="D7" s="30" t="n">
+      <c r="D7" s="31" t="n">
         <v>223</v>
       </c>
     </row>
@@ -17993,13 +18210,13 @@
         <v>102</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>437</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>438</v>
+        <v>430</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>441</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18007,13 +18224,13 @@
         <v>102</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="C9" s="30" t="n">
+        <v>433</v>
+      </c>
+      <c r="C9" s="31" t="n">
         <v>288</v>
       </c>
-      <c r="D9" s="31" t="s">
-        <v>439</v>
+      <c r="D9" s="32" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18021,13 +18238,13 @@
         <v>102</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="C10" s="30" t="n">
+        <v>435</v>
+      </c>
+      <c r="C10" s="31" t="n">
         <v>289</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>440</v>
+      <c r="D10" s="32" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18035,13 +18252,13 @@
         <v>102</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="C11" s="30" t="n">
+        <v>437</v>
+      </c>
+      <c r="C11" s="31" t="n">
         <v>290</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>441</v>
+      <c r="D11" s="32" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18049,12 +18266,12 @@
         <v>102</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="C12" s="30" t="n">
+        <v>439</v>
+      </c>
+      <c r="C12" s="31" t="n">
         <v>291</v>
       </c>
-      <c r="D12" s="31" t="n">
+      <c r="D12" s="32" t="n">
         <v>300</v>
       </c>
     </row>
@@ -18063,12 +18280,12 @@
         <v>102</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="C13" s="30" t="n">
+        <v>440</v>
+      </c>
+      <c r="C13" s="31" t="n">
         <v>292</v>
       </c>
-      <c r="D13" s="31" t="n">
+      <c r="D13" s="32" t="n">
         <v>303</v>
       </c>
     </row>
@@ -18077,13 +18294,13 @@
         <v>74</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>443</v>
+        <v>430</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>446</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18091,13 +18308,13 @@
         <v>74</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="C15" s="30" t="n">
+        <v>433</v>
+      </c>
+      <c r="C15" s="31" t="n">
         <v>272</v>
       </c>
-      <c r="D15" s="31" t="s">
-        <v>444</v>
+      <c r="D15" s="32" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18105,13 +18322,13 @@
         <v>74</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="C16" s="30" t="n">
+        <v>435</v>
+      </c>
+      <c r="C16" s="31" t="n">
         <v>273</v>
       </c>
-      <c r="D16" s="31" t="s">
-        <v>445</v>
+      <c r="D16" s="32" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18119,13 +18336,13 @@
         <v>74</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="C17" s="30" t="n">
+        <v>437</v>
+      </c>
+      <c r="C17" s="31" t="n">
         <v>274</v>
       </c>
-      <c r="D17" s="31" t="s">
-        <v>446</v>
+      <c r="D17" s="32" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18133,12 +18350,12 @@
         <v>74</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="C18" s="30" t="n">
+        <v>439</v>
+      </c>
+      <c r="C18" s="31" t="n">
         <v>275</v>
       </c>
-      <c r="D18" s="31" t="n">
+      <c r="D18" s="32" t="n">
         <v>284</v>
       </c>
     </row>
@@ -18147,12 +18364,12 @@
         <v>74</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="C19" s="30" t="n">
+        <v>440</v>
+      </c>
+      <c r="C19" s="31" t="n">
         <v>276</v>
       </c>
-      <c r="D19" s="31" t="n">
+      <c r="D19" s="32" t="n">
         <v>287</v>
       </c>
     </row>
@@ -19152,11 +19369,11 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="9:9 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.11"/>
@@ -19164,32 +19381,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32" t="s">
-        <v>447</v>
-      </c>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="33" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fix: add more error details
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111OLOMEDIAXXX/Olomedia/oloHealth/V.3.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111OLOMEDIAXXX/Olomedia/oloHealth/V.3.0.0/report-checklist.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="451">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -919,10 +919,7 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.4.4003cd725a780165cde9dbd9892ea3f5411c3b23e99e33e6fc9c81fec848158c.e27e338e40^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">Si e’ verificato un errore imprevisto. Riprovare piu tardi o contattare il supporto tecnico.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'errore viene segnalato all'utente che viene invitato a riprovare o a contattare l'help desk. Il servizio di manutenzione software risolve gli errori giornalmente. Dopo la risoluzione, il medico riprende il processo documentale e invia il documento per la validazione. Se possibile, gli operatori correggono l'errore e ri-validano il documento. Altrimenti, il processo clinico continua e il documento viene rivalidato successivamente. Se il gateway non è disponibile, il documento viene memorizzato e inviato in seguito.</t>
+    <t xml:space="preserve">Tramite una reportistica giornaliera, il servizio di manutenzione software cerchera' di risolvere il problema. Dopo la risoluzione, il medico firmera' il documento e sara' sottoposto alla validazione ed eventuale trasmissione al gateway.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_VPS_CT12_KO</t>
@@ -2177,11 +2174,11 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.89"/>
@@ -3251,11 +3248,11 @@
   </sheetPr>
   <dimension ref="A1:B998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.11"/>
@@ -4358,15 +4355,15 @@
   </sheetPr>
   <dimension ref="A1:T704"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A:A"/>
+      <selection pane="bottomRight" activeCell="P77" activeCellId="0" sqref="P77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.09"/>
@@ -6298,7 +6295,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="27" customFormat="true" ht="131.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="27" t="n">
         <v>128</v>
       </c>
@@ -6330,19 +6327,17 @@
         <v>56</v>
       </c>
       <c r="L45" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="M45" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="N45" s="16" t="s">
-        <v>221</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M45" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="N45" s="16"/>
       <c r="O45" s="27" t="s">
         <v>56</v>
       </c>
       <c r="P45" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q45" s="27" t="s">
         <v>57</v>
@@ -6351,7 +6346,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="27" customFormat="true" ht="145.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="27" t="n">
         <v>129</v>
       </c>
@@ -6362,40 +6357,38 @@
         <v>74</v>
       </c>
       <c r="D46" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E46" s="28" t="s">
         <v>223</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>224</v>
       </c>
       <c r="F46" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G46" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="H46" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="H46" s="27" t="s">
+      <c r="I46" s="27" t="s">
         <v>226</v>
-      </c>
-      <c r="I46" s="27" t="s">
-        <v>227</v>
       </c>
       <c r="J46" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L46" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="M46" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="N46" s="16" t="s">
-        <v>221</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M46" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="N46" s="16"/>
       <c r="O46" s="27" t="s">
         <v>56</v>
       </c>
       <c r="P46" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q46" s="27" t="s">
         <v>57</v>
@@ -6415,22 +6408,22 @@
         <v>74</v>
       </c>
       <c r="D47" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="E47" s="28" t="s">
         <v>228</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>229</v>
       </c>
       <c r="F47" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G47" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="H47" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="H47" s="27" t="s">
+      <c r="I47" s="27" t="s">
         <v>231</v>
-      </c>
-      <c r="I47" s="27" t="s">
-        <v>232</v>
       </c>
       <c r="J47" s="27" t="s">
         <v>56</v>
@@ -6468,22 +6461,22 @@
         <v>74</v>
       </c>
       <c r="D48" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="E48" s="28" t="s">
         <v>233</v>
-      </c>
-      <c r="E48" s="28" t="s">
-        <v>234</v>
       </c>
       <c r="F48" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G48" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="H48" s="27" t="s">
         <v>235</v>
       </c>
-      <c r="H48" s="27" t="s">
+      <c r="I48" s="27" t="s">
         <v>236</v>
-      </c>
-      <c r="I48" s="27" t="s">
-        <v>237</v>
       </c>
       <c r="J48" s="27" t="s">
         <v>56</v>
@@ -6521,22 +6514,22 @@
         <v>74</v>
       </c>
       <c r="D49" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="E49" s="28" t="s">
         <v>238</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>239</v>
       </c>
       <c r="F49" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G49" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="H49" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="H49" s="27" t="s">
+      <c r="I49" s="27" t="s">
         <v>241</v>
-      </c>
-      <c r="I49" s="27" t="s">
-        <v>242</v>
       </c>
       <c r="J49" s="27" t="s">
         <v>56</v>
@@ -6574,22 +6567,22 @@
         <v>74</v>
       </c>
       <c r="D50" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="E50" s="28" t="s">
         <v>243</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>244</v>
       </c>
       <c r="F50" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G50" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="H50" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="H50" s="27" t="s">
+      <c r="I50" s="27" t="s">
         <v>246</v>
-      </c>
-      <c r="I50" s="27" t="s">
-        <v>247</v>
       </c>
       <c r="J50" s="27" t="s">
         <v>56</v>
@@ -6627,22 +6620,22 @@
         <v>74</v>
       </c>
       <c r="D51" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="E51" s="28" t="s">
         <v>248</v>
-      </c>
-      <c r="E51" s="28" t="s">
-        <v>249</v>
       </c>
       <c r="F51" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G51" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="H51" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="H51" s="27" t="s">
+      <c r="I51" s="27" t="s">
         <v>251</v>
-      </c>
-      <c r="I51" s="27" t="s">
-        <v>252</v>
       </c>
       <c r="J51" s="27" t="s">
         <v>56</v>
@@ -6680,22 +6673,22 @@
         <v>74</v>
       </c>
       <c r="D52" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="E52" s="28" t="s">
         <v>253</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>254</v>
       </c>
       <c r="F52" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G52" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="H52" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="H52" s="27" t="s">
+      <c r="I52" s="27" t="s">
         <v>256</v>
-      </c>
-      <c r="I52" s="27" t="s">
-        <v>257</v>
       </c>
       <c r="J52" s="27" t="s">
         <v>56</v>
@@ -6733,22 +6726,22 @@
         <v>74</v>
       </c>
       <c r="D53" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="E53" s="28" t="s">
         <v>258</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>259</v>
       </c>
       <c r="F53" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G53" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="H53" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="H53" s="27" t="s">
+      <c r="I53" s="27" t="s">
         <v>261</v>
-      </c>
-      <c r="I53" s="27" t="s">
-        <v>262</v>
       </c>
       <c r="J53" s="27" t="s">
         <v>56</v>
@@ -6786,22 +6779,22 @@
         <v>74</v>
       </c>
       <c r="D54" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="E54" s="28" t="s">
         <v>263</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>264</v>
       </c>
       <c r="F54" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G54" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="H54" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="H54" s="27" t="s">
+      <c r="I54" s="27" t="s">
         <v>266</v>
-      </c>
-      <c r="I54" s="27" t="s">
-        <v>267</v>
       </c>
       <c r="J54" s="27" t="s">
         <v>56</v>
@@ -6839,22 +6832,22 @@
         <v>74</v>
       </c>
       <c r="D55" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="E55" s="28" t="s">
         <v>268</v>
-      </c>
-      <c r="E55" s="28" t="s">
-        <v>269</v>
       </c>
       <c r="F55" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G55" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="H55" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="H55" s="27" t="s">
+      <c r="I55" s="27" t="s">
         <v>271</v>
-      </c>
-      <c r="I55" s="27" t="s">
-        <v>272</v>
       </c>
       <c r="J55" s="27" t="s">
         <v>56</v>
@@ -6892,22 +6885,22 @@
         <v>74</v>
       </c>
       <c r="D56" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="E56" s="28" t="s">
         <v>273</v>
-      </c>
-      <c r="E56" s="28" t="s">
-        <v>274</v>
       </c>
       <c r="F56" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G56" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="H56" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="H56" s="27" t="s">
+      <c r="I56" s="27" t="s">
         <v>276</v>
-      </c>
-      <c r="I56" s="27" t="s">
-        <v>277</v>
       </c>
       <c r="J56" s="27" t="s">
         <v>56</v>
@@ -6945,22 +6938,22 @@
         <v>74</v>
       </c>
       <c r="D57" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="E57" s="28" t="s">
         <v>278</v>
-      </c>
-      <c r="E57" s="28" t="s">
-        <v>279</v>
       </c>
       <c r="F57" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G57" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="H57" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="H57" s="27" t="s">
+      <c r="I57" s="27" t="s">
         <v>281</v>
-      </c>
-      <c r="I57" s="27" t="s">
-        <v>282</v>
       </c>
       <c r="J57" s="27" t="s">
         <v>56</v>
@@ -6998,22 +6991,22 @@
         <v>74</v>
       </c>
       <c r="D58" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="E58" s="28" t="s">
         <v>283</v>
-      </c>
-      <c r="E58" s="28" t="s">
-        <v>284</v>
       </c>
       <c r="F58" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G58" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="H58" s="27" t="s">
         <v>285</v>
       </c>
-      <c r="H58" s="27" t="s">
+      <c r="I58" s="27" t="s">
         <v>286</v>
-      </c>
-      <c r="I58" s="27" t="s">
-        <v>287</v>
       </c>
       <c r="J58" s="27" t="s">
         <v>56</v>
@@ -7051,22 +7044,22 @@
         <v>74</v>
       </c>
       <c r="D59" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="E59" s="28" t="s">
         <v>288</v>
-      </c>
-      <c r="E59" s="28" t="s">
-        <v>289</v>
       </c>
       <c r="F59" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G59" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="H59" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="H59" s="27" t="s">
+      <c r="I59" s="27" t="s">
         <v>291</v>
-      </c>
-      <c r="I59" s="27" t="s">
-        <v>292</v>
       </c>
       <c r="J59" s="27" t="s">
         <v>56</v>
@@ -7104,22 +7097,22 @@
         <v>74</v>
       </c>
       <c r="D60" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="E60" s="28" t="s">
         <v>293</v>
-      </c>
-      <c r="E60" s="28" t="s">
-        <v>294</v>
       </c>
       <c r="F60" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G60" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="H60" s="27" t="s">
         <v>295</v>
       </c>
-      <c r="H60" s="27" t="s">
+      <c r="I60" s="27" t="s">
         <v>296</v>
-      </c>
-      <c r="I60" s="27" t="s">
-        <v>297</v>
       </c>
       <c r="J60" s="27" t="s">
         <v>56</v>
@@ -7157,22 +7150,22 @@
         <v>74</v>
       </c>
       <c r="D61" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="E61" s="28" t="s">
         <v>298</v>
-      </c>
-      <c r="E61" s="28" t="s">
-        <v>299</v>
       </c>
       <c r="F61" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G61" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="H61" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="H61" s="27" t="s">
+      <c r="I61" s="27" t="s">
         <v>301</v>
-      </c>
-      <c r="I61" s="27" t="s">
-        <v>302</v>
       </c>
       <c r="J61" s="27" t="s">
         <v>56</v>
@@ -7210,22 +7203,22 @@
         <v>74</v>
       </c>
       <c r="D62" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="E62" s="28" t="s">
         <v>303</v>
-      </c>
-      <c r="E62" s="28" t="s">
-        <v>304</v>
       </c>
       <c r="F62" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G62" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="H62" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="H62" s="27" t="s">
+      <c r="I62" s="27" t="s">
         <v>306</v>
-      </c>
-      <c r="I62" s="27" t="s">
-        <v>307</v>
       </c>
       <c r="J62" s="27" t="s">
         <v>56</v>
@@ -7263,22 +7256,22 @@
         <v>74</v>
       </c>
       <c r="D63" s="27" t="s">
+        <v>307</v>
+      </c>
+      <c r="E63" s="28" t="s">
         <v>308</v>
-      </c>
-      <c r="E63" s="28" t="s">
-        <v>309</v>
       </c>
       <c r="F63" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G63" s="27" t="s">
+        <v>309</v>
+      </c>
+      <c r="H63" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="H63" s="27" t="s">
+      <c r="I63" s="27" t="s">
         <v>311</v>
-      </c>
-      <c r="I63" s="27" t="s">
-        <v>312</v>
       </c>
       <c r="J63" s="27" t="s">
         <v>56</v>
@@ -7316,22 +7309,22 @@
         <v>102</v>
       </c>
       <c r="D64" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="E64" s="28" t="s">
         <v>313</v>
-      </c>
-      <c r="E64" s="28" t="s">
-        <v>314</v>
       </c>
       <c r="F64" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G64" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="H64" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="H64" s="27" t="s">
+      <c r="I64" s="27" t="s">
         <v>316</v>
-      </c>
-      <c r="I64" s="27" t="s">
-        <v>317</v>
       </c>
       <c r="J64" s="27" t="s">
         <v>56</v>
@@ -7354,22 +7347,22 @@
         <v>102</v>
       </c>
       <c r="D65" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="E65" s="28" t="s">
         <v>318</v>
-      </c>
-      <c r="E65" s="28" t="s">
-        <v>319</v>
       </c>
       <c r="F65" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G65" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="H65" s="27" t="s">
         <v>320</v>
       </c>
-      <c r="H65" s="27" t="s">
+      <c r="I65" s="27" t="s">
         <v>321</v>
-      </c>
-      <c r="I65" s="27" t="s">
-        <v>322</v>
       </c>
       <c r="J65" s="27" t="s">
         <v>56</v>
@@ -7392,22 +7385,22 @@
         <v>102</v>
       </c>
       <c r="D66" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="E66" s="28" t="s">
         <v>323</v>
-      </c>
-      <c r="E66" s="28" t="s">
-        <v>324</v>
       </c>
       <c r="F66" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G66" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="H66" s="27" t="s">
         <v>325</v>
       </c>
-      <c r="H66" s="27" t="s">
+      <c r="I66" s="27" t="s">
         <v>326</v>
-      </c>
-      <c r="I66" s="27" t="s">
-        <v>327</v>
       </c>
       <c r="J66" s="27" t="s">
         <v>56</v>
@@ -7430,22 +7423,22 @@
         <v>102</v>
       </c>
       <c r="D67" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="E67" s="28" t="s">
         <v>328</v>
-      </c>
-      <c r="E67" s="28" t="s">
-        <v>329</v>
       </c>
       <c r="F67" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G67" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="H67" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="H67" s="27" t="s">
+      <c r="I67" s="27" t="s">
         <v>331</v>
-      </c>
-      <c r="I67" s="27" t="s">
-        <v>332</v>
       </c>
       <c r="J67" s="27" t="s">
         <v>56</v>
@@ -7468,22 +7461,22 @@
         <v>102</v>
       </c>
       <c r="D68" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="E68" s="28" t="s">
         <v>333</v>
-      </c>
-      <c r="E68" s="28" t="s">
-        <v>334</v>
       </c>
       <c r="F68" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G68" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="H68" s="27" t="s">
         <v>335</v>
       </c>
-      <c r="H68" s="27" t="s">
+      <c r="I68" s="27" t="s">
         <v>336</v>
-      </c>
-      <c r="I68" s="27" t="s">
-        <v>337</v>
       </c>
       <c r="J68" s="27" t="s">
         <v>56</v>
@@ -7494,7 +7487,7 @@
       <c r="M68" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="N68" s="30" t="s">
+      <c r="N68" s="14" t="s">
         <v>129</v>
       </c>
       <c r="O68" s="27" t="s">
@@ -7521,22 +7514,22 @@
         <v>102</v>
       </c>
       <c r="D69" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="E69" s="28" t="s">
         <v>338</v>
-      </c>
-      <c r="E69" s="28" t="s">
-        <v>339</v>
       </c>
       <c r="F69" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G69" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="H69" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="H69" s="27" t="s">
+      <c r="I69" s="27" t="s">
         <v>341</v>
-      </c>
-      <c r="I69" s="27" t="s">
-        <v>342</v>
       </c>
       <c r="J69" s="27" t="s">
         <v>56</v>
@@ -7574,22 +7567,22 @@
         <v>102</v>
       </c>
       <c r="D70" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="E70" s="28" t="s">
         <v>343</v>
-      </c>
-      <c r="E70" s="28" t="s">
-        <v>344</v>
       </c>
       <c r="F70" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G70" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="H70" s="27" t="s">
         <v>345</v>
       </c>
-      <c r="H70" s="27" t="s">
+      <c r="I70" s="27" t="s">
         <v>346</v>
-      </c>
-      <c r="I70" s="27" t="s">
-        <v>347</v>
       </c>
       <c r="J70" s="27" t="s">
         <v>56</v>
@@ -7627,22 +7620,22 @@
         <v>102</v>
       </c>
       <c r="D71" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="E71" s="28" t="s">
         <v>348</v>
-      </c>
-      <c r="E71" s="28" t="s">
-        <v>349</v>
       </c>
       <c r="F71" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G71" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="H71" s="27" t="s">
         <v>350</v>
       </c>
-      <c r="H71" s="27" t="s">
+      <c r="I71" s="27" t="s">
         <v>351</v>
-      </c>
-      <c r="I71" s="27" t="s">
-        <v>352</v>
       </c>
       <c r="J71" s="27" t="s">
         <v>56</v>
@@ -7680,22 +7673,22 @@
         <v>102</v>
       </c>
       <c r="D72" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="E72" s="28" t="s">
         <v>353</v>
-      </c>
-      <c r="E72" s="28" t="s">
-        <v>354</v>
       </c>
       <c r="F72" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G72" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="H72" s="27" t="s">
         <v>355</v>
       </c>
-      <c r="H72" s="27" t="s">
+      <c r="I72" s="27" t="s">
         <v>356</v>
-      </c>
-      <c r="I72" s="27" t="s">
-        <v>357</v>
       </c>
       <c r="J72" s="27" t="s">
         <v>56</v>
@@ -7733,22 +7726,22 @@
         <v>102</v>
       </c>
       <c r="D73" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="E73" s="28" t="s">
         <v>358</v>
-      </c>
-      <c r="E73" s="28" t="s">
-        <v>359</v>
       </c>
       <c r="F73" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G73" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="H73" s="27" t="s">
         <v>360</v>
       </c>
-      <c r="H73" s="27" t="s">
+      <c r="I73" s="27" t="s">
         <v>361</v>
-      </c>
-      <c r="I73" s="27" t="s">
-        <v>362</v>
       </c>
       <c r="J73" s="27" t="s">
         <v>56</v>
@@ -7775,7 +7768,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" s="27" customFormat="true" ht="145.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="27" t="n">
         <v>157</v>
       </c>
@@ -7786,40 +7779,38 @@
         <v>102</v>
       </c>
       <c r="D74" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="E74" s="28" t="s">
         <v>363</v>
-      </c>
-      <c r="E74" s="28" t="s">
-        <v>364</v>
       </c>
       <c r="F74" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G74" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="H74" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="H74" s="27" t="s">
+      <c r="I74" s="27" t="s">
         <v>366</v>
-      </c>
-      <c r="I74" s="27" t="s">
-        <v>367</v>
       </c>
       <c r="J74" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L74" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="M74" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="N74" s="16" t="s">
-        <v>221</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M74" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="N74" s="16"/>
       <c r="O74" s="27" t="s">
         <v>56</v>
       </c>
       <c r="P74" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q74" s="27" t="s">
         <v>57</v>
@@ -7839,22 +7830,22 @@
         <v>102</v>
       </c>
       <c r="D75" s="27" t="s">
+        <v>367</v>
+      </c>
+      <c r="E75" s="28" t="s">
         <v>368</v>
-      </c>
-      <c r="E75" s="28" t="s">
-        <v>369</v>
       </c>
       <c r="F75" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G75" s="27" t="s">
+        <v>369</v>
+      </c>
+      <c r="H75" s="27" t="s">
         <v>370</v>
       </c>
-      <c r="H75" s="27" t="s">
+      <c r="I75" s="27" t="s">
         <v>371</v>
-      </c>
-      <c r="I75" s="27" t="s">
-        <v>372</v>
       </c>
       <c r="J75" s="27" t="s">
         <v>56</v>
@@ -7881,7 +7872,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="76" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" s="27" customFormat="true" ht="131.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="27" t="n">
         <v>159</v>
       </c>
@@ -7892,40 +7883,38 @@
         <v>102</v>
       </c>
       <c r="D76" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="E76" s="28" t="s">
         <v>373</v>
-      </c>
-      <c r="E76" s="28" t="s">
-        <v>374</v>
       </c>
       <c r="F76" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G76" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="H76" s="27" t="s">
         <v>375</v>
       </c>
-      <c r="H76" s="27" t="s">
+      <c r="I76" s="27" t="s">
         <v>376</v>
-      </c>
-      <c r="I76" s="27" t="s">
-        <v>377</v>
       </c>
       <c r="J76" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L76" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="M76" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="N76" s="16" t="s">
-        <v>221</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M76" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="N76" s="16"/>
       <c r="O76" s="27" t="s">
         <v>56</v>
       </c>
       <c r="P76" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q76" s="27" t="s">
         <v>57</v>
@@ -7934,7 +7923,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="77" s="27" customFormat="true" ht="161.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" s="27" customFormat="true" ht="131.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="27" t="n">
         <v>160</v>
       </c>
@@ -7945,40 +7934,38 @@
         <v>102</v>
       </c>
       <c r="D77" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="E77" s="28" t="s">
         <v>378</v>
-      </c>
-      <c r="E77" s="28" t="s">
-        <v>379</v>
       </c>
       <c r="F77" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G77" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="H77" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="H77" s="27" t="s">
+      <c r="I77" s="27" t="s">
         <v>381</v>
-      </c>
-      <c r="I77" s="27" t="s">
-        <v>382</v>
       </c>
       <c r="J77" s="27" t="s">
         <v>56</v>
       </c>
       <c r="L77" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="M77" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="N77" s="16" t="s">
-        <v>221</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M77" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="N77" s="16"/>
       <c r="O77" s="27" t="s">
         <v>56</v>
       </c>
       <c r="P77" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q77" s="27" t="s">
         <v>57</v>
@@ -7998,22 +7985,22 @@
         <v>102</v>
       </c>
       <c r="D78" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="E78" s="28" t="s">
         <v>383</v>
-      </c>
-      <c r="E78" s="28" t="s">
-        <v>384</v>
       </c>
       <c r="F78" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G78" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="H78" s="27" t="s">
         <v>385</v>
       </c>
-      <c r="H78" s="27" t="s">
+      <c r="I78" s="27" t="s">
         <v>386</v>
-      </c>
-      <c r="I78" s="27" t="s">
-        <v>387</v>
       </c>
       <c r="J78" s="27" t="s">
         <v>56</v>
@@ -8051,22 +8038,22 @@
         <v>102</v>
       </c>
       <c r="D79" s="27" t="s">
+        <v>387</v>
+      </c>
+      <c r="E79" s="28" t="s">
         <v>388</v>
-      </c>
-      <c r="E79" s="28" t="s">
-        <v>389</v>
       </c>
       <c r="F79" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G79" s="27" t="s">
+        <v>389</v>
+      </c>
+      <c r="H79" s="27" t="s">
         <v>390</v>
       </c>
-      <c r="H79" s="27" t="s">
+      <c r="I79" s="27" t="s">
         <v>391</v>
-      </c>
-      <c r="I79" s="27" t="s">
-        <v>392</v>
       </c>
       <c r="J79" s="27" t="s">
         <v>56</v>
@@ -8104,22 +8091,22 @@
         <v>102</v>
       </c>
       <c r="D80" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E80" s="28" t="s">
         <v>393</v>
-      </c>
-      <c r="E80" s="28" t="s">
-        <v>394</v>
       </c>
       <c r="F80" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G80" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="H80" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="H80" s="27" t="s">
+      <c r="I80" s="27" t="s">
         <v>396</v>
-      </c>
-      <c r="I80" s="27" t="s">
-        <v>397</v>
       </c>
       <c r="J80" s="27" t="s">
         <v>56</v>
@@ -8157,22 +8144,22 @@
         <v>102</v>
       </c>
       <c r="D81" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="E81" s="28" t="s">
         <v>398</v>
-      </c>
-      <c r="E81" s="28" t="s">
-        <v>399</v>
       </c>
       <c r="F81" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G81" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="H81" s="27" t="s">
         <v>400</v>
       </c>
-      <c r="H81" s="27" t="s">
+      <c r="I81" s="27" t="s">
         <v>401</v>
-      </c>
-      <c r="I81" s="27" t="s">
-        <v>402</v>
       </c>
       <c r="J81" s="27" t="s">
         <v>56</v>
@@ -8210,22 +8197,22 @@
         <v>102</v>
       </c>
       <c r="D82" s="27" t="s">
+        <v>402</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>403</v>
-      </c>
-      <c r="E82" s="28" t="s">
-        <v>404</v>
       </c>
       <c r="F82" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G82" s="27" t="s">
+        <v>404</v>
+      </c>
+      <c r="H82" s="27" t="s">
         <v>405</v>
       </c>
-      <c r="H82" s="27" t="s">
+      <c r="I82" s="27" t="s">
         <v>406</v>
-      </c>
-      <c r="I82" s="27" t="s">
-        <v>407</v>
       </c>
       <c r="J82" s="27" t="s">
         <v>56</v>
@@ -8263,22 +8250,22 @@
         <v>102</v>
       </c>
       <c r="D83" s="27" t="s">
+        <v>407</v>
+      </c>
+      <c r="E83" s="28" t="s">
         <v>408</v>
-      </c>
-      <c r="E83" s="28" t="s">
-        <v>409</v>
       </c>
       <c r="F83" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G83" s="27" t="s">
+        <v>409</v>
+      </c>
+      <c r="H83" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="H83" s="27" t="s">
+      <c r="I83" s="27" t="s">
         <v>411</v>
-      </c>
-      <c r="I83" s="27" t="s">
-        <v>412</v>
       </c>
       <c r="J83" s="27" t="s">
         <v>56</v>
@@ -8316,22 +8303,22 @@
         <v>102</v>
       </c>
       <c r="D84" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="E84" s="28" t="s">
         <v>413</v>
-      </c>
-      <c r="E84" s="28" t="s">
-        <v>414</v>
       </c>
       <c r="F84" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G84" s="27" t="s">
+        <v>414</v>
+      </c>
+      <c r="H84" s="27" t="s">
         <v>415</v>
       </c>
-      <c r="H84" s="27" t="s">
+      <c r="I84" s="27" t="s">
         <v>416</v>
-      </c>
-      <c r="I84" s="27" t="s">
-        <v>417</v>
       </c>
       <c r="J84" s="27" t="s">
         <v>56</v>
@@ -8369,22 +8356,22 @@
         <v>102</v>
       </c>
       <c r="D85" s="27" t="s">
+        <v>417</v>
+      </c>
+      <c r="E85" s="28" t="s">
         <v>418</v>
-      </c>
-      <c r="E85" s="28" t="s">
-        <v>419</v>
       </c>
       <c r="F85" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G85" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="H85" s="27" t="s">
         <v>420</v>
       </c>
-      <c r="H85" s="27" t="s">
+      <c r="I85" s="27" t="s">
         <v>421</v>
-      </c>
-      <c r="I85" s="27" t="s">
-        <v>422</v>
       </c>
       <c r="J85" s="27" t="s">
         <v>56</v>
@@ -8422,22 +8409,22 @@
         <v>102</v>
       </c>
       <c r="D86" s="27" t="s">
+        <v>422</v>
+      </c>
+      <c r="E86" s="28" t="s">
         <v>423</v>
-      </c>
-      <c r="E86" s="28" t="s">
-        <v>424</v>
       </c>
       <c r="F86" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G86" s="27" t="s">
+        <v>424</v>
+      </c>
+      <c r="H86" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="H86" s="27" t="s">
+      <c r="I86" s="27" t="s">
         <v>426</v>
-      </c>
-      <c r="I86" s="27" t="s">
-        <v>427</v>
       </c>
       <c r="J86" s="27" t="s">
         <v>56</v>
@@ -18090,13 +18077,13 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.87"/>
@@ -18115,10 +18102,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>428</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18126,13 +18113,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>430</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="D2" s="31" t="s">
         <v>431</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18140,13 +18127,13 @@
         <v>49</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C3" s="31" t="n">
         <v>208</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18154,13 +18141,13 @@
         <v>49</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C4" s="31" t="n">
         <v>209</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18168,13 +18155,13 @@
         <v>49</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C5" s="31" t="n">
         <v>210</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18182,7 +18169,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C6" s="31" t="n">
         <v>211</v>
@@ -18196,7 +18183,7 @@
         <v>49</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C7" s="31" t="n">
         <v>212</v>
@@ -18210,13 +18197,13 @@
         <v>102</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C8" s="31" t="s">
+        <v>440</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>441</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18224,13 +18211,13 @@
         <v>102</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C9" s="31" t="n">
         <v>288</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18238,13 +18225,13 @@
         <v>102</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C10" s="31" t="n">
         <v>289</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18252,13 +18239,13 @@
         <v>102</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C11" s="31" t="n">
         <v>290</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18266,7 +18253,7 @@
         <v>102</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C12" s="31" t="n">
         <v>291</v>
@@ -18280,7 +18267,7 @@
         <v>102</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C13" s="31" t="n">
         <v>292</v>
@@ -18294,13 +18281,13 @@
         <v>74</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C14" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="D14" s="32" t="s">
         <v>446</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18308,13 +18295,13 @@
         <v>74</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C15" s="31" t="n">
         <v>272</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18322,13 +18309,13 @@
         <v>74</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C16" s="31" t="n">
         <v>273</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18336,13 +18323,13 @@
         <v>74</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C17" s="31" t="n">
         <v>274</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18350,7 +18337,7 @@
         <v>74</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C18" s="31" t="n">
         <v>275</v>
@@ -18364,7 +18351,7 @@
         <v>74</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C19" s="31" t="n">
         <v>276</v>
@@ -19369,11 +19356,11 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.11"/>
@@ -19398,7 +19385,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>99</v>

</xml_diff>